<commit_message>
More doc work, added focus group suggestions to product backlog
</commit_message>
<xml_diff>
--- a/docs/deliverable2/Getana_Deliverable_2_SprintBacklog_2.xlsx
+++ b/docs/deliverable2/Getana_Deliverable_2_SprintBacklog_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brodywilliams/Repositories/RaiderNAV/docs/deliverable2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB30CEB-7C44-FE4E-A7C9-DD120BB6AE82}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B747C19-FCC2-4445-B093-D5B2984AA424}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18300" windowHeight="18000" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="18300" windowHeight="16460" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -274,9 +274,6 @@
     <t>45, Update daily scrum report</t>
   </si>
   <si>
-    <t xml:space="preserve">In progess as of end of sprint </t>
-  </si>
-  <si>
     <t>Arpit: 100%</t>
   </si>
   <si>
@@ -287,6 +284,9 @@
   </si>
   <si>
     <t>Yong, Vasilis, Arpit, Michael, Sakshyam, Brody: 100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In progress as of end of sprint </t>
   </si>
 </sst>
 </file>
@@ -1341,7 +1341,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1492,7 +1492,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -1510,7 +1510,7 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.15">
@@ -1645,10 +1645,10 @@
         <v>4</v>
       </c>
       <c r="F20" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.15">
@@ -1668,10 +1668,10 @@
         <v>4</v>
       </c>
       <c r="F21" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.15">
@@ -1691,10 +1691,10 @@
         <v>4</v>
       </c>
       <c r="F22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" t="s">
         <v>82</v>
-      </c>
-      <c r="G22" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.15">
@@ -1714,7 +1714,7 @@
         <v>4</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="G23" t="s">
         <v>25</v>

</xml_diff>